<commit_message>
Additions and changes made
-Added a readme
-removed manual control buttons as they are not required
-attempting to change project names
</commit_message>
<xml_diff>
--- a/Documentation/Testing.xlsx
+++ b/Documentation/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA3E926-5333-4A0B-AA07-33217CF1CC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838FCB14-986A-42B8-ACAB-CA13FB8DCBF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,12 +114,6 @@
     <t>Client Controller greenhouse data request data button</t>
   </si>
   <si>
-    <t>connect button should be disabled if the input is anything other than full stops or numbers.</t>
-  </si>
-  <si>
-    <t>The input box should disable the server connect button on any input that is not a full stop or a number to prevent the controller client from trying to connect to a bad address.</t>
-  </si>
-  <si>
     <t>the port input should disable the server connect button on any input that is nota number to prevent the controller client from trying to connect to a bad port.</t>
   </si>
   <si>
@@ -271,6 +265,19 @@
   </si>
   <si>
     <t>Request Handler</t>
+  </si>
+  <si>
+    <t>Connection attempt should not be started and appropriate message should be displayed in the status text box if the IP address is invalid.
+If the ip address is valid the Controller client should connect to the server.</t>
+  </si>
+  <si>
+    <t>Tests all the possible inputs. When 'Connect' button is pressed, the connection attempt should not go through on invalid ip address input. Ip Address is invalidated if:
+1. Any characters other than numbers and full stops are present
+2. IP address does not begin or end with a number
+3. IP address has more than 4 sets of numbers or 3 full stops between the numbers
+4. IP address has more than one consecutive dots
+5. A number set converted into an integer is not between 0 and 255
+6. More than three characters numbers per number set are present</t>
   </si>
 </sst>
 </file>
@@ -631,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +648,7 @@
     <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="83.5703125" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -673,7 +680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -681,11 +688,12 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -695,10 +703,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -706,13 +714,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -723,10 +731,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -737,10 +745,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -751,10 +759,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -765,10 +773,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -779,10 +787,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -793,10 +801,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -807,10 +815,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -821,10 +829,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -835,10 +843,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -849,10 +857,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -863,10 +871,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -877,10 +885,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -891,10 +899,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -905,10 +913,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -919,10 +927,10 @@
         <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -933,10 +941,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -947,10 +955,10 @@
         <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -961,10 +969,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -975,10 +983,10 @@
         <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -986,18 +994,18 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="2"/>
     </row>
@@ -1036,22 +1044,22 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>